<commit_message>
Final additions & official figures
</commit_message>
<xml_diff>
--- a/data/PCR_16S_LABELS.xlsx
+++ b/data/PCR_16S_LABELS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabriela.acevedo/Documents/git_repos/oystersedseq_grao_2022/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FCD21E73-63A6-A746-97EF-5B692FCDC6FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE148E43-8ACD-2844-AE1E-6B0B93969BBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15900" xr2:uid="{DD566E8F-94BC-5C43-82A2-1E8C39405795}"/>
   </bookViews>
@@ -321,12 +321,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -341,9 +347,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -661,7 +668,7 @@
   <dimension ref="A1:B43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -682,7 +689,7 @@
       <c r="A2" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -690,7 +697,7 @@
       <c r="A3" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -730,7 +737,7 @@
       <c r="A8" t="s">
         <v>47</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -738,7 +745,7 @@
       <c r="A9" t="s">
         <v>48</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -778,7 +785,7 @@
       <c r="A14" t="s">
         <v>53</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="2" t="s">
         <v>14</v>
       </c>
     </row>
@@ -786,7 +793,7 @@
       <c r="A15" t="s">
         <v>54</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="2" t="s">
         <v>15</v>
       </c>
     </row>
@@ -818,7 +825,7 @@
       <c r="A19" t="s">
         <v>58</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -826,7 +833,7 @@
       <c r="A20" t="s">
         <v>59</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="2" t="s">
         <v>20</v>
       </c>
     </row>
@@ -858,7 +865,7 @@
       <c r="A24" t="s">
         <v>63</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="2" t="s">
         <v>24</v>
       </c>
     </row>
@@ -866,7 +873,7 @@
       <c r="A25" t="s">
         <v>67</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -898,7 +905,7 @@
       <c r="A29" t="s">
         <v>68</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="2" t="s">
         <v>29</v>
       </c>
     </row>
@@ -938,7 +945,7 @@
       <c r="A34" t="s">
         <v>73</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" s="2" t="s">
         <v>34</v>
       </c>
     </row>
@@ -978,7 +985,7 @@
       <c r="A39" t="s">
         <v>78</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B39" s="2" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>